<commit_message>
made JfreeApache and updated other programs with correct smoother, remade outputs
</commit_message>
<xml_diff>
--- a/Project 2/Documents/FunctionPlotterDocuments/SalterOutput/output1SaltedGraph.xlsx
+++ b/Project 2/Documents/FunctionPlotterDocuments/SalterOutput/output1SaltedGraph.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rance\OneDrive\Documents\My Files\Other\College Class Materials\ThirdYearSpring\Probability and Applied Statistics\Projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1866C303-B62D-4AF9-BFE7-1123BB2C0B41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E260FA22-18CC-4455-A7CD-F46681F4A5B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{28540048-0324-4202-9FE6-045ADBE1C1C3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{93AADB2A-DB24-469B-8CD6-8ACE599D5A00}"/>
   </bookViews>
   <sheets>
     <sheet name="output1Salted" sheetId="1" r:id="rId1"/>
@@ -592,14 +592,16 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Salted Output</a:t>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Salted Output (Range: 10 - 50)</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> (Range: 10 - 50)</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -979,304 +981,304 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
                 <c:pt idx="0">
-                  <c:v>-39</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>46</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>46</c:v>
+                  <c:v>-21</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>56</c:v>
+                  <c:v>-28</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-12</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>79</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>35</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>31</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>121</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>115</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>135</c:v>
+                  <c:v>108</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>125</c:v>
+                  <c:v>177</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>198</c:v>
+                  <c:v>124</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>170</c:v>
+                  <c:v>224</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>187</c:v>
+                  <c:v>212</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>288</c:v>
+                  <c:v>284</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>266</c:v>
+                  <c:v>321</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>369</c:v>
+                  <c:v>281</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>385</c:v>
+                  <c:v>334</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>420</c:v>
+                  <c:v>365</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>477</c:v>
+                  <c:v>461</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>523</c:v>
+                  <c:v>445</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>499</c:v>
+                  <c:v>506</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>538</c:v>
+                  <c:v>549</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>653</c:v>
+                  <c:v>657</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>643</c:v>
+                  <c:v>696</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>743</c:v>
+                  <c:v>691</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>817</c:v>
+                  <c:v>803</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>882</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>865</c:v>
+                  <c:v>926</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>953</c:v>
+                  <c:v>941</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1060</c:v>
+                  <c:v>979</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1072</c:v>
+                  <c:v>1063</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1173</c:v>
+                  <c:v>1202</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1270</c:v>
+                  <c:v>1263</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1334</c:v>
+                  <c:v>1264</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1403</c:v>
+                  <c:v>1335</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1466</c:v>
+                  <c:v>1478</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1551</c:v>
+                  <c:v>1565</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1630</c:v>
+                  <c:v>1640</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1665</c:v>
+                  <c:v>1725</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1736</c:v>
+                  <c:v>1731</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1803</c:v>
+                  <c:v>1838</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1896</c:v>
+                  <c:v>1964</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2043</c:v>
+                  <c:v>2071</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>2107</c:v>
+                  <c:v>2152</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>2162</c:v>
+                  <c:v>2245</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>2345</c:v>
+                  <c:v>2350</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>2360</c:v>
+                  <c:v>2450</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>2461</c:v>
+                  <c:v>2518</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>2587</c:v>
+                  <c:v>2579</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>2731</c:v>
+                  <c:v>2730</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>2848</c:v>
+                  <c:v>2775</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>2900</c:v>
+                  <c:v>2932</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>3043</c:v>
+                  <c:v>3017</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>3174</c:v>
+                  <c:v>3089</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>3232</c:v>
+                  <c:v>3265</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>3318</c:v>
+                  <c:v>3323</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>3437</c:v>
+                  <c:v>3525</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>3569</c:v>
+                  <c:v>3564</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>3742</c:v>
+                  <c:v>3690</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>3856</c:v>
+                  <c:v>3802</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>3936</c:v>
+                  <c:v>3994</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>4056</c:v>
+                  <c:v>4076</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>4257</c:v>
+                  <c:v>4239</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>4386</c:v>
+                  <c:v>4338</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>4539</c:v>
+                  <c:v>4444</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>4645</c:v>
+                  <c:v>4669</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>4733</c:v>
+                  <c:v>4794</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>4867</c:v>
+                  <c:v>4881</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>5011</c:v>
+                  <c:v>5072</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>5151</c:v>
+                  <c:v>5221</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>5364</c:v>
+                  <c:v>5318</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>5524</c:v>
+                  <c:v>5449</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>5578</c:v>
+                  <c:v>5615</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>5794</c:v>
+                  <c:v>5761</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>5975</c:v>
+                  <c:v>5920</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>6108</c:v>
+                  <c:v>6128</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>6262</c:v>
+                  <c:v>6292</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>6364</c:v>
+                  <c:v>6362</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>6523</c:v>
+                  <c:v>6586</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>6772</c:v>
+                  <c:v>6771</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>6921</c:v>
+                  <c:v>6935</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>7042</c:v>
+                  <c:v>7026</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>7250</c:v>
+                  <c:v>7268</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>7379</c:v>
+                  <c:v>7364</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>7603</c:v>
+                  <c:v>7540</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>7717</c:v>
+                  <c:v>7700</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>7900</c:v>
+                  <c:v>7895</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>8074</c:v>
+                  <c:v>8140</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>8312</c:v>
+                  <c:v>8296</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>8478</c:v>
+                  <c:v>8450</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>8638</c:v>
+                  <c:v>8680</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>8872</c:v>
+                  <c:v>8799</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>9063</c:v>
+                  <c:v>8991</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>9203</c:v>
+                  <c:v>9264</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>9446</c:v>
+                  <c:v>9422</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>9573</c:v>
+                  <c:v>9567</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>9819</c:v>
+                  <c:v>9784</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>9967</c:v>
+                  <c:v>10028</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1284,7 +1286,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-B6BC-4399-8526-C8DA0425D7C7}"/>
+              <c16:uniqueId val="{00000000-A495-40E5-81A1-8C16296D9614}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1296,11 +1298,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2142388127"/>
-        <c:axId val="2142389087"/>
+        <c:axId val="1755324432"/>
+        <c:axId val="1755323472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2142388127"/>
+        <c:axId val="1755324432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1340,7 +1342,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
                   <a:t>X-Values</a:t>
                 </a:r>
               </a:p>
@@ -1412,12 +1421,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2142389087"/>
+        <c:crossAx val="1755323472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2142389087"/>
+        <c:axId val="1755323472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1457,7 +1466,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
                   <a:t>Y-Values</a:t>
                 </a:r>
               </a:p>
@@ -1529,7 +1545,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2142388127"/>
+        <c:crossAx val="1755324432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2139,22 +2155,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:colOff>99060</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBF29EA2-44A6-1727-00F7-526414167FC9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B93E007B-A6E2-DF2A-3987-89A6D5EA9AD3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2491,11 +2507,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20B31363-738E-4DB7-BC25-91AE4F65879A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8E46E5C-60F0-4A52-A03C-A1F870AB0E7D}">
   <dimension ref="A1:B100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2505,7 +2521,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>-39</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -2513,7 +2529,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>46</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -2521,7 +2537,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>46</v>
+        <v>-21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -2529,7 +2545,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>56</v>
+        <v>-28</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -2537,7 +2553,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>-12</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -2545,7 +2561,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>79</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -2553,7 +2569,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>35</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -2561,7 +2577,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>31</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -2569,7 +2585,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>121</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -2577,7 +2593,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>115</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -2585,7 +2601,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>135</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -2593,7 +2609,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>125</v>
+        <v>177</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -2601,7 +2617,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>198</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -2609,7 +2625,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>170</v>
+        <v>224</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -2617,7 +2633,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>187</v>
+        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -2625,7 +2641,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -2633,7 +2649,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>266</v>
+        <v>321</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -2641,7 +2657,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>369</v>
+        <v>281</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -2649,7 +2665,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>385</v>
+        <v>334</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -2657,7 +2673,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>420</v>
+        <v>365</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -2665,7 +2681,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>477</v>
+        <v>461</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -2673,7 +2689,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>523</v>
+        <v>445</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -2681,7 +2697,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>499</v>
+        <v>506</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -2689,7 +2705,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>538</v>
+        <v>549</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -2697,7 +2713,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>653</v>
+        <v>657</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -2705,7 +2721,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>643</v>
+        <v>696</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -2713,7 +2729,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>743</v>
+        <v>691</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -2721,7 +2737,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>817</v>
+        <v>803</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -2737,7 +2753,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>865</v>
+        <v>926</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -2745,7 +2761,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>953</v>
+        <v>941</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -2753,7 +2769,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>1060</v>
+        <v>979</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -2761,7 +2777,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>1072</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -2769,7 +2785,7 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>1173</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -2777,7 +2793,7 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>1270</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -2785,7 +2801,7 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>1334</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -2793,7 +2809,7 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>1403</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -2801,7 +2817,7 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>1466</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -2809,7 +2825,7 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>1551</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -2817,7 +2833,7 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>1630</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -2825,7 +2841,7 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>1665</v>
+        <v>1725</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -2833,7 +2849,7 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>1736</v>
+        <v>1731</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -2841,7 +2857,7 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>1803</v>
+        <v>1838</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
@@ -2849,7 +2865,7 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>1896</v>
+        <v>1964</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -2857,7 +2873,7 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>2043</v>
+        <v>2071</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
@@ -2865,7 +2881,7 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>2107</v>
+        <v>2152</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -2873,7 +2889,7 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>2162</v>
+        <v>2245</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
@@ -2881,7 +2897,7 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>2345</v>
+        <v>2350</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -2889,7 +2905,7 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>2360</v>
+        <v>2450</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
@@ -2897,7 +2913,7 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>2461</v>
+        <v>2518</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
@@ -2905,7 +2921,7 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>2587</v>
+        <v>2579</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
@@ -2913,7 +2929,7 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>2731</v>
+        <v>2730</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
@@ -2921,7 +2937,7 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>2848</v>
+        <v>2775</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
@@ -2929,7 +2945,7 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>2900</v>
+        <v>2932</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
@@ -2937,7 +2953,7 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>3043</v>
+        <v>3017</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
@@ -2945,7 +2961,7 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>3174</v>
+        <v>3089</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
@@ -2953,7 +2969,7 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>3232</v>
+        <v>3265</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
@@ -2961,7 +2977,7 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>3318</v>
+        <v>3323</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
@@ -2969,7 +2985,7 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>3437</v>
+        <v>3525</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
@@ -2977,7 +2993,7 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>3569</v>
+        <v>3564</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
@@ -2985,7 +3001,7 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>3742</v>
+        <v>3690</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
@@ -2993,7 +3009,7 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <v>3856</v>
+        <v>3802</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
@@ -3001,7 +3017,7 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <v>3936</v>
+        <v>3994</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
@@ -3009,7 +3025,7 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <v>4056</v>
+        <v>4076</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
@@ -3017,7 +3033,7 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <v>4257</v>
+        <v>4239</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
@@ -3025,7 +3041,7 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <v>4386</v>
+        <v>4338</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
@@ -3033,7 +3049,7 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <v>4539</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
@@ -3041,7 +3057,7 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <v>4645</v>
+        <v>4669</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
@@ -3049,7 +3065,7 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <v>4733</v>
+        <v>4794</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
@@ -3057,7 +3073,7 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <v>4867</v>
+        <v>4881</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
@@ -3065,7 +3081,7 @@
         <v>70</v>
       </c>
       <c r="B71">
-        <v>5011</v>
+        <v>5072</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
@@ -3073,7 +3089,7 @@
         <v>71</v>
       </c>
       <c r="B72">
-        <v>5151</v>
+        <v>5221</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
@@ -3081,7 +3097,7 @@
         <v>72</v>
       </c>
       <c r="B73">
-        <v>5364</v>
+        <v>5318</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
@@ -3089,7 +3105,7 @@
         <v>73</v>
       </c>
       <c r="B74">
-        <v>5524</v>
+        <v>5449</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
@@ -3097,7 +3113,7 @@
         <v>74</v>
       </c>
       <c r="B75">
-        <v>5578</v>
+        <v>5615</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
@@ -3105,7 +3121,7 @@
         <v>75</v>
       </c>
       <c r="B76">
-        <v>5794</v>
+        <v>5761</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
@@ -3113,7 +3129,7 @@
         <v>76</v>
       </c>
       <c r="B77">
-        <v>5975</v>
+        <v>5920</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
@@ -3121,7 +3137,7 @@
         <v>77</v>
       </c>
       <c r="B78">
-        <v>6108</v>
+        <v>6128</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
@@ -3129,7 +3145,7 @@
         <v>78</v>
       </c>
       <c r="B79">
-        <v>6262</v>
+        <v>6292</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
@@ -3137,7 +3153,7 @@
         <v>79</v>
       </c>
       <c r="B80">
-        <v>6364</v>
+        <v>6362</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
@@ -3145,7 +3161,7 @@
         <v>80</v>
       </c>
       <c r="B81">
-        <v>6523</v>
+        <v>6586</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
@@ -3153,7 +3169,7 @@
         <v>81</v>
       </c>
       <c r="B82">
-        <v>6772</v>
+        <v>6771</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
@@ -3161,7 +3177,7 @@
         <v>82</v>
       </c>
       <c r="B83">
-        <v>6921</v>
+        <v>6935</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
@@ -3169,7 +3185,7 @@
         <v>83</v>
       </c>
       <c r="B84">
-        <v>7042</v>
+        <v>7026</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
@@ -3177,7 +3193,7 @@
         <v>84</v>
       </c>
       <c r="B85">
-        <v>7250</v>
+        <v>7268</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
@@ -3185,7 +3201,7 @@
         <v>85</v>
       </c>
       <c r="B86">
-        <v>7379</v>
+        <v>7364</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
@@ -3193,7 +3209,7 @@
         <v>86</v>
       </c>
       <c r="B87">
-        <v>7603</v>
+        <v>7540</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
@@ -3201,7 +3217,7 @@
         <v>87</v>
       </c>
       <c r="B88">
-        <v>7717</v>
+        <v>7700</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
@@ -3209,7 +3225,7 @@
         <v>88</v>
       </c>
       <c r="B89">
-        <v>7900</v>
+        <v>7895</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
@@ -3217,7 +3233,7 @@
         <v>89</v>
       </c>
       <c r="B90">
-        <v>8074</v>
+        <v>8140</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
@@ -3225,7 +3241,7 @@
         <v>90</v>
       </c>
       <c r="B91">
-        <v>8312</v>
+        <v>8296</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
@@ -3233,7 +3249,7 @@
         <v>91</v>
       </c>
       <c r="B92">
-        <v>8478</v>
+        <v>8450</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
@@ -3241,7 +3257,7 @@
         <v>92</v>
       </c>
       <c r="B93">
-        <v>8638</v>
+        <v>8680</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
@@ -3249,7 +3265,7 @@
         <v>93</v>
       </c>
       <c r="B94">
-        <v>8872</v>
+        <v>8799</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
@@ -3257,7 +3273,7 @@
         <v>94</v>
       </c>
       <c r="B95">
-        <v>9063</v>
+        <v>8991</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
@@ -3265,7 +3281,7 @@
         <v>95</v>
       </c>
       <c r="B96">
-        <v>9203</v>
+        <v>9264</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
@@ -3273,7 +3289,7 @@
         <v>96</v>
       </c>
       <c r="B97">
-        <v>9446</v>
+        <v>9422</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
@@ -3281,7 +3297,7 @@
         <v>97</v>
       </c>
       <c r="B98">
-        <v>9573</v>
+        <v>9567</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
@@ -3289,7 +3305,7 @@
         <v>98</v>
       </c>
       <c r="B99">
-        <v>9819</v>
+        <v>9784</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
@@ -3297,7 +3313,7 @@
         <v>99</v>
       </c>
       <c r="B100">
-        <v>9967</v>
+        <v>10028</v>
       </c>
     </row>
   </sheetData>

</xml_diff>